<commit_message>
A1#111ELIOSSUITEXX: Accreditamento RAD+RSA+LDO+LAB - Corr. Checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/EliosSuite/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/EliosSuite/3/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FSE2_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse_git\it-fse-accreditamento\GATEWAY\A1#111ELIOSSUITEXX\eliossuite\EliosSuite\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277704F7-7B42-49BF-83DE-8A893FDB07A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BC6661-86E5-4CEC-8626-355791F041FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2695" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="1043">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4899,6 +4899,9 @@
   <si>
     <t xml:space="preserve">Non viene gestita la sezione
 </t>
+  </si>
+  <si>
+    <t>non gestito</t>
   </si>
 </sst>
 </file>
@@ -7855,10 +7858,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T10" sqref="T10"/>
+      <selection pane="bottomRight" activeCell="B383" sqref="B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -15738,8 +15741,12 @@
       <c r="G198" s="24"/>
       <c r="H198" s="24"/>
       <c r="I198" s="24"/>
-      <c r="J198" s="25"/>
-      <c r="K198" s="25"/>
+      <c r="J198" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="K198" s="25" t="s">
+        <v>1042</v>
+      </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
       <c r="N198" s="25"/>
@@ -22068,8 +22075,12 @@
       <c r="G383" s="24"/>
       <c r="H383" s="24"/>
       <c r="I383" s="24"/>
-      <c r="J383" s="25"/>
-      <c r="K383" s="25"/>
+      <c r="J383" s="25" t="s">
+        <v>841</v>
+      </c>
+      <c r="K383" s="25" t="s">
+        <v>1042</v>
+      </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>
       <c r="N383" s="25"/>

</xml_diff>

<commit_message>
A1#111ELIOSSUITEXX: Accreditamento RAD+RSA+LDO+LAB - Corr. Segnalazioni
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/EliosSuite/3/report-checklist.xlsx
+++ b/GATEWAY/A1#111ELIOSSUITEXX/eliossuite/EliosSuite/3/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fse_git\it-fse-accreditamento\GATEWAY\A1#111ELIOSSUITEXX\eliossuite\EliosSuite\3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\FSE2_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BC6661-86E5-4CEC-8626-355791F041FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB479E33-5044-4AF3-BBD0-418A49A16BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2699" uniqueCount="1043">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="1041">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4302,24 +4302,6 @@
     <t>e8c1de7ddae6442c</t>
   </si>
   <si>
-    <t>2024-04-30T11:23:10:00Z</t>
-  </si>
-  <si>
-    <t>4228af37290268a3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.0f4c2d5961a5575988a270d51b46b05de096f9badfe158b62dee535a5130c06c.93614b635f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-04-30T11:25:33:00Z</t>
-  </si>
-  <si>
-    <t>a820c7d1df3ae1c4</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.0f4c2d5961a5575988a270d51b46b05de096f9badfe158b62dee535a5130c06c.fd4ed974c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-04-30T11:58:50:00Z</t>
   </si>
   <si>
@@ -4483,24 +4465,6 @@
     <t>062296d5899de242</t>
   </si>
   <si>
-    <t>2024-05-02T10:23:32:00Z</t>
-  </si>
-  <si>
-    <t>d24be9e55688ea54</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.28a304a70d33473003851f932b522112d41ae54170179cd4be64502d2d6f61a6.7da42f27d3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-05-02T11:08:36:00Z</t>
-  </si>
-  <si>
-    <t>25ae8e61691fb16b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.28a304a70d33473003851f932b522112d41ae54170179cd4be64502d2d6f61a6.fc4a066db1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-05-02T11:40:42:00Z</t>
   </si>
   <si>
@@ -4765,24 +4729,6 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.54f95249b186a381047a1d805b6d316f4de1f5909d80f8069c947fc1717797f9.036ec2f5fe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2024-05-08T11:11:42:00Z</t>
-  </si>
-  <si>
-    <t>af4f6417d410c742</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.66e0d9b209669242af6ac80122211ca626414e5681350bd406ef9fa9d8688e95.753081bf95^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-05-08T11:15:16:00Z</t>
-  </si>
-  <si>
-    <t>1e33c3756222ef0f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.66e0d9b209669242af6ac80122211ca626414e5681350bd406ef9fa9d8688e95.3909c32c60^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2024-05-08T11:16:21:00Z</t>
   </si>
   <si>
@@ -4901,7 +4847,56 @@
 </t>
   </si>
   <si>
-    <t>non gestito</t>
+    <t>2024-05-22T09:36:55:00Z</t>
+  </si>
+  <si>
+    <t>e3aefecc9cf5bc37</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.0f4c2d5961a5575988a270d51b46b05de096f9badfe158b62dee535a5130c06c.edf78ecd77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-22T09:40:37:00Z</t>
+  </si>
+  <si>
+    <t>8f06a73eb075e02a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.0f4c2d5961a5575988a270d51b46b05de096f9badfe158b62dee535a5130c06c.9e263a755e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-22T10:12:21:00Z</t>
+  </si>
+  <si>
+    <t>f77c8686b1101cd5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.28a304a70d33473003851f932b522112d41ae54170179cd4be64502d2d6f61a6.698d7ae634^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Non gestita</t>
+  </si>
+  <si>
+    <t>2024-05-22T10:16:44:00Z</t>
+  </si>
+  <si>
+    <t>403877719fdded15</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.28a304a70d33473003851f932b522112d41ae54170179cd4be64502d2d6f61a6.00d9c08193^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-05-22T11:41:15:00Z</t>
+  </si>
+  <si>
+    <t>d33b05be19a15019</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.66e0d9b209669242af6ac80122211ca626414e5681350bd406ef9fa9d8688e95.c97a140fe8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non viene gestita la sezione partecipant
+</t>
   </si>
 </sst>
 </file>
@@ -5718,7 +5713,7 @@
     </row>
     <row r="4" spans="1:1" ht="14.25" customHeight="1">
       <c r="A4" s="42" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="14.25" customHeight="1">
@@ -7858,10 +7853,10 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B165" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B383" sqref="B383"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7928,7 +7923,7 @@
       </c>
       <c r="B3" s="52"/>
       <c r="C3" s="57" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="D3" s="49"/>
       <c r="F3" s="12"/>
@@ -7951,7 +7946,7 @@
       <c r="A4" s="53"/>
       <c r="B4" s="54"/>
       <c r="C4" s="57" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="4"/>
@@ -7975,7 +7970,7 @@
       <c r="A5" s="55"/>
       <c r="B5" s="56"/>
       <c r="C5" s="57" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="D5" s="49"/>
       <c r="F5" s="12"/>
@@ -8130,16 +8125,16 @@
         <v>46</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>991</v>
+        <v>979</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>991</v>
+        <v>979</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>992</v>
+        <v>980</v>
       </c>
       <c r="I10" s="33" t="s">
-        <v>993</v>
+        <v>981</v>
       </c>
       <c r="J10" s="34" t="s">
         <v>132</v>
@@ -8174,16 +8169,16 @@
         <v>49</v>
       </c>
       <c r="F11" s="33" t="s">
-        <v>994</v>
+        <v>982</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>994</v>
+        <v>982</v>
       </c>
       <c r="H11" s="33" t="s">
-        <v>995</v>
+        <v>983</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>996</v>
+        <v>984</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>132</v>
@@ -8218,16 +8213,16 @@
         <v>51</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>997</v>
+        <v>1037</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>997</v>
+        <v>1037</v>
       </c>
       <c r="H12" s="33" t="s">
-        <v>998</v>
+        <v>1038</v>
       </c>
       <c r="I12" s="33" t="s">
-        <v>999</v>
+        <v>1039</v>
       </c>
       <c r="J12" s="34" t="s">
         <v>132</v>
@@ -8269,7 +8264,7 @@
         <v>841</v>
       </c>
       <c r="K13" s="45" t="s">
-        <v>1041</v>
+        <v>1023</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -8299,22 +8294,16 @@
       <c r="E14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="33" t="s">
-        <v>1000</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>1000</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>1001</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>1002</v>
-      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
       <c r="J14" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="25"/>
+        <v>841</v>
+      </c>
+      <c r="K14" s="45" t="s">
+        <v>1040</v>
+      </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
@@ -8351,7 +8340,7 @@
         <v>841</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
@@ -8389,7 +8378,7 @@
         <v>841</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -8427,7 +8416,7 @@
         <v>841</v>
       </c>
       <c r="K17" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -8465,7 +8454,7 @@
         <v>841</v>
       </c>
       <c r="K18" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -8496,16 +8485,16 @@
         <v>67</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>850</v>
+        <v>1027</v>
       </c>
       <c r="G19" s="36" t="s">
-        <v>850</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>851</v>
+        <v>1027</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>1028</v>
       </c>
       <c r="I19" s="33" t="s">
-        <v>852</v>
+        <v>1029</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>132</v>
@@ -8540,16 +8529,16 @@
         <v>69</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>132</v>
@@ -8591,7 +8580,7 @@
         <v>841</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -8629,7 +8618,7 @@
         <v>841</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -9068,13 +9057,13 @@
         <v>102</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
       <c r="H35" s="33" t="s">
-        <v>1004</v>
+        <v>986</v>
       </c>
       <c r="I35" s="33" t="s">
         <v>842</v>
@@ -9090,13 +9079,13 @@
         <v>132</v>
       </c>
       <c r="N35" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O35" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P35" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q35" s="25"/>
       <c r="R35" s="26"/>
@@ -9122,13 +9111,13 @@
         <v>102</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>961</v>
+        <v>949</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>961</v>
+        <v>949</v>
       </c>
       <c r="H36" s="33" t="s">
-        <v>960</v>
+        <v>948</v>
       </c>
       <c r="I36" s="33" t="s">
         <v>842</v>
@@ -9144,13 +9133,13 @@
         <v>132</v>
       </c>
       <c r="N36" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O36" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P36" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q36" s="25"/>
       <c r="R36" s="26"/>
@@ -9232,13 +9221,13 @@
         <v>132</v>
       </c>
       <c r="N38" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O38" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P38" s="34" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="Q38" s="25"/>
       <c r="R38" s="26"/>
@@ -9264,13 +9253,13 @@
         <v>102</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="G39" s="33" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="I39" s="33" t="s">
         <v>842</v>
@@ -9286,13 +9275,13 @@
         <v>132</v>
       </c>
       <c r="N39" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O39" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P39" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q39" s="25"/>
       <c r="R39" s="26"/>
@@ -9420,13 +9409,13 @@
         <v>118</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>1005</v>
+        <v>987</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>1005</v>
+        <v>987</v>
       </c>
       <c r="H43" s="33" t="s">
-        <v>1006</v>
+        <v>988</v>
       </c>
       <c r="I43" s="33" t="s">
         <v>842</v>
@@ -9442,13 +9431,13 @@
         <v>132</v>
       </c>
       <c r="N43" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O43" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P43" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q43" s="25"/>
       <c r="R43" s="26"/>
@@ -9474,13 +9463,13 @@
         <v>118</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>962</v>
+        <v>950</v>
       </c>
       <c r="G44" s="33" t="s">
-        <v>962</v>
+        <v>950</v>
       </c>
       <c r="H44" s="33" t="s">
-        <v>963</v>
+        <v>951</v>
       </c>
       <c r="I44" s="33" t="s">
         <v>842</v>
@@ -9496,13 +9485,13 @@
         <v>132</v>
       </c>
       <c r="N44" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O44" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P44" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q44" s="25"/>
       <c r="R44" s="26"/>
@@ -9582,13 +9571,13 @@
         <v>132</v>
       </c>
       <c r="N46" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O46" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P46" s="34" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -9614,13 +9603,13 @@
         <v>118</v>
       </c>
       <c r="F47" s="33" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="G47" s="33" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="H47" s="33" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="I47" s="33" t="s">
         <v>842</v>
@@ -9636,13 +9625,13 @@
         <v>132</v>
       </c>
       <c r="N47" s="34" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="O47" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>951</v>
+        <v>939</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -9784,13 +9773,13 @@
         <v>132</v>
       </c>
       <c r="N51" s="34" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="O51" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P51" s="34" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="Q51" s="25"/>
       <c r="R51" s="26" t="s">
@@ -9832,13 +9821,13 @@
         <v>132</v>
       </c>
       <c r="N52" s="34" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="O52" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P52" s="34" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="Q52" s="25"/>
       <c r="R52" s="26" t="s">
@@ -9916,13 +9905,13 @@
         <v>132</v>
       </c>
       <c r="N54" s="34" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="O54" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P54" s="41" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="Q54" s="25"/>
       <c r="R54" s="26" t="s">
@@ -9964,13 +9953,13 @@
         <v>132</v>
       </c>
       <c r="N55" s="34" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="O55" s="34" t="s">
         <v>132</v>
       </c>
       <c r="P55" s="34" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="Q55" s="25"/>
       <c r="R55" s="26" t="s">
@@ -10106,16 +10095,16 @@
         <v>141</v>
       </c>
       <c r="F59" s="33" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="G59" s="33" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="H59" s="33" t="s">
-        <v>1008</v>
+        <v>990</v>
       </c>
       <c r="I59" s="33" t="s">
-        <v>1009</v>
+        <v>991</v>
       </c>
       <c r="J59" s="34" t="s">
         <v>132</v>
@@ -10128,13 +10117,13 @@
         <v>132</v>
       </c>
       <c r="N59" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O59" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P59" s="34" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
       <c r="Q59" s="25"/>
       <c r="R59" s="26"/>
@@ -10160,16 +10149,16 @@
         <v>143</v>
       </c>
       <c r="F60" s="33" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="H60" s="33" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
       <c r="I60" s="33" t="s">
-        <v>1012</v>
+        <v>994</v>
       </c>
       <c r="J60" s="34" t="s">
         <v>132</v>
@@ -10182,13 +10171,13 @@
         <v>132</v>
       </c>
       <c r="N60" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O60" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P60" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q60" s="25"/>
       <c r="R60" s="26"/>
@@ -10214,16 +10203,16 @@
         <v>145</v>
       </c>
       <c r="F61" s="33" t="s">
-        <v>1013</v>
+        <v>995</v>
       </c>
       <c r="G61" s="33" t="s">
-        <v>1013</v>
+        <v>995</v>
       </c>
       <c r="H61" s="33" t="s">
-        <v>1014</v>
+        <v>996</v>
       </c>
       <c r="I61" s="33" t="s">
-        <v>1015</v>
+        <v>997</v>
       </c>
       <c r="J61" s="34" t="s">
         <v>132</v>
@@ -10236,13 +10225,13 @@
         <v>132</v>
       </c>
       <c r="N61" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O61" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P61" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="26"/>
@@ -10268,16 +10257,16 @@
         <v>147</v>
       </c>
       <c r="F62" s="33" t="s">
-        <v>1016</v>
+        <v>998</v>
       </c>
       <c r="G62" s="33" t="s">
-        <v>1016</v>
+        <v>998</v>
       </c>
       <c r="H62" s="33" t="s">
-        <v>1017</v>
+        <v>999</v>
       </c>
       <c r="I62" s="33" t="s">
-        <v>1018</v>
+        <v>1000</v>
       </c>
       <c r="J62" s="34" t="s">
         <v>132</v>
@@ -10290,13 +10279,13 @@
         <v>132</v>
       </c>
       <c r="N62" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O62" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P62" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="26"/>
@@ -10322,16 +10311,16 @@
         <v>149</v>
       </c>
       <c r="F63" s="33" t="s">
-        <v>1019</v>
+        <v>1001</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>1019</v>
+        <v>1001</v>
       </c>
       <c r="H63" s="33" t="s">
-        <v>1020</v>
+        <v>1002</v>
       </c>
       <c r="I63" s="33" t="s">
-        <v>1021</v>
+        <v>1003</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>132</v>
@@ -10344,13 +10333,13 @@
         <v>132</v>
       </c>
       <c r="N63" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O63" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P63" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q63" s="25"/>
       <c r="R63" s="26"/>
@@ -10376,16 +10365,16 @@
         <v>151</v>
       </c>
       <c r="F64" s="33" t="s">
-        <v>1022</v>
+        <v>1004</v>
       </c>
       <c r="G64" s="33" t="s">
-        <v>1022</v>
+        <v>1004</v>
       </c>
       <c r="H64" s="33" t="s">
-        <v>1023</v>
+        <v>1005</v>
       </c>
       <c r="I64" s="33" t="s">
-        <v>1024</v>
+        <v>1006</v>
       </c>
       <c r="J64" s="34" t="s">
         <v>132</v>
@@ -10398,13 +10387,13 @@
         <v>132</v>
       </c>
       <c r="N64" s="34" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="O64" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P64" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q64" s="25"/>
       <c r="R64" s="26"/>
@@ -10430,16 +10419,16 @@
         <v>153</v>
       </c>
       <c r="F65" s="33" t="s">
-        <v>1025</v>
+        <v>1007</v>
       </c>
       <c r="G65" s="33" t="s">
-        <v>1025</v>
+        <v>1007</v>
       </c>
       <c r="H65" s="33" t="s">
-        <v>1026</v>
+        <v>1008</v>
       </c>
       <c r="I65" s="33" t="s">
-        <v>1027</v>
+        <v>1009</v>
       </c>
       <c r="J65" s="34" t="s">
         <v>132</v>
@@ -10452,13 +10441,13 @@
         <v>132</v>
       </c>
       <c r="N65" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O65" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P65" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q65" s="25"/>
       <c r="R65" s="26"/>
@@ -10484,16 +10473,16 @@
         <v>155</v>
       </c>
       <c r="F66" s="33" t="s">
-        <v>1028</v>
+        <v>1010</v>
       </c>
       <c r="G66" s="33" t="s">
-        <v>1028</v>
+        <v>1010</v>
       </c>
       <c r="H66" s="33" t="s">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="I66" s="33" t="s">
-        <v>1030</v>
+        <v>1012</v>
       </c>
       <c r="J66" s="34" t="s">
         <v>132</v>
@@ -10506,13 +10495,13 @@
         <v>132</v>
       </c>
       <c r="N66" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O66" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P66" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q66" s="25"/>
       <c r="R66" s="26"/>
@@ -10538,16 +10527,16 @@
         <v>157</v>
       </c>
       <c r="F67" s="33" t="s">
-        <v>1031</v>
+        <v>1013</v>
       </c>
       <c r="G67" s="33" t="s">
-        <v>1031</v>
+        <v>1013</v>
       </c>
       <c r="H67" s="33" t="s">
-        <v>1032</v>
+        <v>1014</v>
       </c>
       <c r="I67" s="33" t="s">
-        <v>1033</v>
+        <v>1015</v>
       </c>
       <c r="J67" s="34" t="s">
         <v>132</v>
@@ -10560,13 +10549,13 @@
         <v>132</v>
       </c>
       <c r="N67" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O67" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P67" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="26"/>
@@ -10592,16 +10581,16 @@
         <v>159</v>
       </c>
       <c r="F68" s="33" t="s">
-        <v>1034</v>
+        <v>1016</v>
       </c>
       <c r="G68" s="33" t="s">
-        <v>1034</v>
+        <v>1016</v>
       </c>
       <c r="H68" s="33" t="s">
-        <v>1035</v>
+        <v>1017</v>
       </c>
       <c r="I68" s="33" t="s">
-        <v>1036</v>
+        <v>1018</v>
       </c>
       <c r="J68" s="34" t="s">
         <v>132</v>
@@ -10614,13 +10603,13 @@
         <v>132</v>
       </c>
       <c r="N68" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O68" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P68" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="26"/>
@@ -10646,16 +10635,16 @@
         <v>161</v>
       </c>
       <c r="F69" s="33" t="s">
-        <v>1037</v>
+        <v>1019</v>
       </c>
       <c r="G69" s="33" t="s">
-        <v>1037</v>
+        <v>1019</v>
       </c>
       <c r="H69" s="33" t="s">
-        <v>1038</v>
+        <v>1020</v>
       </c>
       <c r="I69" s="33" t="s">
-        <v>1039</v>
+        <v>1021</v>
       </c>
       <c r="J69" s="34" t="s">
         <v>132</v>
@@ -10668,13 +10657,13 @@
         <v>132</v>
       </c>
       <c r="N69" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O69" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P69" s="34" t="s">
-        <v>1040</v>
+        <v>1022</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="26"/>
@@ -10700,16 +10689,16 @@
         <v>163</v>
       </c>
       <c r="F70" s="33" t="s">
-        <v>964</v>
+        <v>952</v>
       </c>
       <c r="G70" s="33" t="s">
-        <v>964</v>
+        <v>952</v>
       </c>
       <c r="H70" s="33" t="s">
-        <v>965</v>
+        <v>953</v>
       </c>
       <c r="I70" s="33" t="s">
-        <v>966</v>
+        <v>954</v>
       </c>
       <c r="J70" s="34" t="s">
         <v>132</v>
@@ -10722,13 +10711,13 @@
         <v>132</v>
       </c>
       <c r="N70" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O70" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P70" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q70" s="25"/>
       <c r="R70" s="26"/>
@@ -10754,16 +10743,16 @@
         <v>165</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>967</v>
+        <v>955</v>
       </c>
       <c r="G71" s="33" t="s">
-        <v>967</v>
+        <v>955</v>
       </c>
       <c r="H71" s="33" t="s">
-        <v>968</v>
+        <v>956</v>
       </c>
       <c r="I71" s="33" t="s">
-        <v>969</v>
+        <v>957</v>
       </c>
       <c r="J71" s="34" t="s">
         <v>132</v>
@@ -10776,13 +10765,13 @@
         <v>132</v>
       </c>
       <c r="N71" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O71" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P71" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q71" s="25"/>
       <c r="R71" s="26"/>
@@ -10808,16 +10797,16 @@
         <v>167</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>970</v>
+        <v>958</v>
       </c>
       <c r="G72" s="33" t="s">
-        <v>970</v>
+        <v>958</v>
       </c>
       <c r="H72" s="33" t="s">
-        <v>971</v>
+        <v>959</v>
       </c>
       <c r="I72" s="33" t="s">
-        <v>972</v>
+        <v>960</v>
       </c>
       <c r="J72" s="34" t="s">
         <v>132</v>
@@ -10830,13 +10819,13 @@
         <v>132</v>
       </c>
       <c r="N72" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O72" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P72" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q72" s="25"/>
       <c r="R72" s="26"/>
@@ -10862,16 +10851,16 @@
         <v>169</v>
       </c>
       <c r="F73" s="33" t="s">
-        <v>973</v>
+        <v>961</v>
       </c>
       <c r="G73" s="33" t="s">
-        <v>973</v>
+        <v>961</v>
       </c>
       <c r="H73" s="33" t="s">
-        <v>974</v>
+        <v>962</v>
       </c>
       <c r="I73" s="33" t="s">
-        <v>975</v>
+        <v>963</v>
       </c>
       <c r="J73" s="34" t="s">
         <v>132</v>
@@ -10884,13 +10873,13 @@
         <v>132</v>
       </c>
       <c r="N73" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O73" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P73" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q73" s="25"/>
       <c r="R73" s="26"/>
@@ -10916,16 +10905,16 @@
         <v>171</v>
       </c>
       <c r="F74" s="33" t="s">
-        <v>976</v>
+        <v>964</v>
       </c>
       <c r="G74" s="33" t="s">
-        <v>976</v>
+        <v>964</v>
       </c>
       <c r="H74" s="33" t="s">
-        <v>977</v>
+        <v>965</v>
       </c>
       <c r="I74" s="33" t="s">
-        <v>978</v>
+        <v>966</v>
       </c>
       <c r="J74" s="34" t="s">
         <v>132</v>
@@ -10938,13 +10927,13 @@
         <v>132</v>
       </c>
       <c r="N74" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O74" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P74" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q74" s="25"/>
       <c r="R74" s="26"/>
@@ -10970,16 +10959,16 @@
         <v>173</v>
       </c>
       <c r="F75" s="33" t="s">
-        <v>979</v>
+        <v>967</v>
       </c>
       <c r="G75" s="33" t="s">
-        <v>979</v>
+        <v>967</v>
       </c>
       <c r="H75" s="33" t="s">
-        <v>980</v>
+        <v>968</v>
       </c>
       <c r="I75" s="33" t="s">
-        <v>981</v>
+        <v>969</v>
       </c>
       <c r="J75" s="34" t="s">
         <v>132</v>
@@ -10992,13 +10981,13 @@
         <v>132</v>
       </c>
       <c r="N75" s="34" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="O75" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P75" s="34" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
       <c r="Q75" s="25"/>
       <c r="R75" s="26"/>
@@ -11024,16 +11013,16 @@
         <v>175</v>
       </c>
       <c r="F76" s="33" t="s">
-        <v>982</v>
+        <v>970</v>
       </c>
       <c r="G76" s="33" t="s">
-        <v>982</v>
+        <v>970</v>
       </c>
       <c r="H76" s="33" t="s">
-        <v>983</v>
+        <v>971</v>
       </c>
       <c r="I76" s="33" t="s">
-        <v>984</v>
+        <v>972</v>
       </c>
       <c r="J76" s="34" t="s">
         <v>132</v>
@@ -11046,13 +11035,13 @@
         <v>132</v>
       </c>
       <c r="N76" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O76" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P76" s="34" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="Q76" s="25"/>
       <c r="R76" s="26"/>
@@ -11078,16 +11067,16 @@
         <v>177</v>
       </c>
       <c r="F77" s="33" t="s">
-        <v>985</v>
+        <v>973</v>
       </c>
       <c r="G77" s="33" t="s">
-        <v>985</v>
+        <v>973</v>
       </c>
       <c r="H77" s="33" t="s">
-        <v>986</v>
+        <v>974</v>
       </c>
       <c r="I77" s="33" t="s">
-        <v>987</v>
+        <v>975</v>
       </c>
       <c r="J77" s="34" t="s">
         <v>132</v>
@@ -11100,13 +11089,13 @@
         <v>132</v>
       </c>
       <c r="N77" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O77" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P77" s="34" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="Q77" s="25"/>
       <c r="R77" s="26"/>
@@ -11139,7 +11128,7 @@
         <v>841</v>
       </c>
       <c r="K78" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
@@ -11177,7 +11166,7 @@
         <v>841</v>
       </c>
       <c r="K79" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L79" s="25"/>
       <c r="M79" s="25"/>
@@ -11215,7 +11204,7 @@
         <v>841</v>
       </c>
       <c r="K80" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L80" s="25"/>
       <c r="M80" s="25"/>
@@ -11253,7 +11242,7 @@
         <v>841</v>
       </c>
       <c r="K81" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L81" s="25"/>
       <c r="M81" s="25"/>
@@ -11284,16 +11273,16 @@
         <v>187</v>
       </c>
       <c r="F82" s="36" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="G82" s="36" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="H82" s="36" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="I82" s="33" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="J82" s="34" t="s">
         <v>132</v>
@@ -11306,13 +11295,13 @@
         <v>132</v>
       </c>
       <c r="N82" s="43" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O82" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P82" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q82" s="25"/>
       <c r="R82" s="26"/>
@@ -11338,16 +11327,16 @@
         <v>189</v>
       </c>
       <c r="F83" s="39" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="G83" s="33" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="H83" s="33" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="I83" s="33" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>132</v>
@@ -11360,13 +11349,13 @@
         <v>132</v>
       </c>
       <c r="N83" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O83" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P83" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q83" s="25"/>
       <c r="R83" s="26"/>
@@ -11392,16 +11381,16 @@
         <v>191</v>
       </c>
       <c r="F84" s="33" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="G84" s="33" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="H84" s="33" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="I84" s="33" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="J84" s="34" t="s">
         <v>132</v>
@@ -11414,13 +11403,13 @@
         <v>132</v>
       </c>
       <c r="N84" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O84" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P84" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q84" s="25"/>
       <c r="R84" s="26"/>
@@ -11446,16 +11435,16 @@
         <v>193</v>
       </c>
       <c r="F85" s="33" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="G85" s="33" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="H85" s="33" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="I85" s="33" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="J85" s="34" t="s">
         <v>132</v>
@@ -11468,13 +11457,13 @@
         <v>132</v>
       </c>
       <c r="N85" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O85" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P85" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q85" s="25"/>
       <c r="R85" s="26"/>
@@ -11500,16 +11489,16 @@
         <v>195</v>
       </c>
       <c r="F86" s="33" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="G86" s="33" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="H86" s="33" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="I86" s="33" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="J86" s="34" t="s">
         <v>132</v>
@@ -11522,13 +11511,13 @@
         <v>132</v>
       </c>
       <c r="N86" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O86" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P86" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q86" s="25"/>
       <c r="R86" s="26"/>
@@ -11554,16 +11543,16 @@
         <v>197</v>
       </c>
       <c r="F87" s="33" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="G87" s="33" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="H87" s="33" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="I87" s="33" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="J87" s="34" t="s">
         <v>132</v>
@@ -11576,13 +11565,13 @@
         <v>132</v>
       </c>
       <c r="N87" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O87" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P87" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q87" s="25"/>
       <c r="R87" s="26"/>
@@ -11615,7 +11604,7 @@
         <v>841</v>
       </c>
       <c r="K88" s="34" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="L88" s="25"/>
       <c r="M88" s="25"/>
@@ -11653,7 +11642,7 @@
         <v>841</v>
       </c>
       <c r="K89" s="34" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="L89" s="25"/>
       <c r="M89" s="25"/>
@@ -11684,16 +11673,16 @@
         <v>203</v>
       </c>
       <c r="F90" s="33" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="G90" s="33" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="H90" s="33" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="I90" s="33" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="J90" s="34" t="s">
         <v>132</v>
@@ -11706,13 +11695,13 @@
         <v>132</v>
       </c>
       <c r="N90" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O90" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P90" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q90" s="25"/>
       <c r="R90" s="26"/>
@@ -11738,16 +11727,16 @@
         <v>205</v>
       </c>
       <c r="F91" s="33" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="G91" s="33" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="H91" s="33" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="I91" s="33" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="J91" s="34" t="s">
         <v>132</v>
@@ -11760,13 +11749,13 @@
         <v>132</v>
       </c>
       <c r="N91" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O91" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P91" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q91" s="25"/>
       <c r="R91" s="26"/>
@@ -11792,16 +11781,16 @@
         <v>207</v>
       </c>
       <c r="F92" s="33" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="G92" s="33" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="H92" s="33" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="I92" s="33" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="J92" s="34" t="s">
         <v>132</v>
@@ -11814,13 +11803,13 @@
         <v>132</v>
       </c>
       <c r="N92" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O92" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P92" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q92" s="25"/>
       <c r="R92" s="26"/>
@@ -11853,7 +11842,7 @@
         <v>841</v>
       </c>
       <c r="K93" s="34" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="L93" s="25"/>
       <c r="M93" s="25"/>
@@ -11891,7 +11880,7 @@
         <v>841</v>
       </c>
       <c r="K94" s="34" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="L94" s="25"/>
       <c r="M94" s="25"/>
@@ -11926,10 +11915,10 @@
       <c r="H95" s="38"/>
       <c r="I95" s="24"/>
       <c r="J95" s="34" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="K95" s="34" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="L95" s="25"/>
       <c r="M95" s="25"/>
@@ -11967,7 +11956,7 @@
         <v>841</v>
       </c>
       <c r="K96" s="34" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="L96" s="25"/>
       <c r="M96" s="25"/>
@@ -12002,10 +11991,10 @@
       <c r="H97" s="38"/>
       <c r="I97" s="24"/>
       <c r="J97" s="34" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="K97" s="34" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="L97" s="25"/>
       <c r="M97" s="25"/>
@@ -12040,10 +12029,10 @@
       <c r="H98" s="38"/>
       <c r="I98" s="24"/>
       <c r="J98" s="34" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="K98" s="34" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="L98" s="25"/>
       <c r="M98" s="25"/>
@@ -12081,7 +12070,7 @@
         <v>841</v>
       </c>
       <c r="K99" s="34" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="L99" s="25"/>
       <c r="M99" s="25"/>
@@ -12119,7 +12108,7 @@
         <v>841</v>
       </c>
       <c r="K100" s="34" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="L100" s="25"/>
       <c r="M100" s="25"/>
@@ -13952,16 +13941,16 @@
         <v>331</v>
       </c>
       <c r="F154" s="33" t="s">
-        <v>907</v>
+        <v>1034</v>
       </c>
       <c r="G154" s="33" t="s">
-        <v>907</v>
+        <v>1034</v>
       </c>
       <c r="H154" s="33" t="s">
-        <v>908</v>
+        <v>1035</v>
       </c>
       <c r="I154" s="33" t="s">
-        <v>909</v>
+        <v>1036</v>
       </c>
       <c r="J154" s="34" t="s">
         <v>132</v>
@@ -14003,7 +13992,7 @@
         <v>841</v>
       </c>
       <c r="K155" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L155" s="25"/>
       <c r="M155" s="25"/>
@@ -14041,7 +14030,7 @@
         <v>841</v>
       </c>
       <c r="K156" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L156" s="25"/>
       <c r="M156" s="25"/>
@@ -14079,7 +14068,7 @@
         <v>841</v>
       </c>
       <c r="K157" s="44" t="s">
-        <v>946</v>
+        <v>934</v>
       </c>
       <c r="L157" s="25"/>
       <c r="M157" s="25"/>
@@ -14110,16 +14099,16 @@
         <v>339</v>
       </c>
       <c r="F158" s="33" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="G158" s="33" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="H158" s="33" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="I158" s="33" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="J158" s="34" t="s">
         <v>132</v>
@@ -14132,13 +14121,13 @@
         <v>132</v>
       </c>
       <c r="N158" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O158" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P158" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q158" s="25"/>
       <c r="R158" s="26"/>
@@ -14164,16 +14153,16 @@
         <v>341</v>
       </c>
       <c r="F159" s="33" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="G159" s="33" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="H159" s="33" t="s">
-        <v>914</v>
+        <v>902</v>
       </c>
       <c r="I159" s="33" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
       <c r="J159" s="34" t="s">
         <v>132</v>
@@ -14186,13 +14175,13 @@
         <v>132</v>
       </c>
       <c r="N159" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O159" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P159" s="34" t="s">
-        <v>952</v>
+        <v>940</v>
       </c>
       <c r="Q159" s="25"/>
       <c r="R159" s="26"/>
@@ -14218,16 +14207,16 @@
         <v>343</v>
       </c>
       <c r="F160" s="33" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="G160" s="33" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="H160" s="33" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="I160" s="33" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
       <c r="J160" s="34" t="s">
         <v>132</v>
@@ -14240,13 +14229,13 @@
         <v>132</v>
       </c>
       <c r="N160" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O160" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P160" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q160" s="25"/>
       <c r="R160" s="26"/>
@@ -14272,16 +14261,16 @@
         <v>345</v>
       </c>
       <c r="F161" s="33" t="s">
-        <v>919</v>
+        <v>907</v>
       </c>
       <c r="G161" s="33" t="s">
-        <v>919</v>
+        <v>907</v>
       </c>
       <c r="H161" s="33" t="s">
-        <v>920</v>
+        <v>908</v>
       </c>
       <c r="I161" s="33" t="s">
-        <v>921</v>
+        <v>909</v>
       </c>
       <c r="J161" s="34" t="s">
         <v>132</v>
@@ -14294,13 +14283,13 @@
         <v>132</v>
       </c>
       <c r="N161" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O161" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P161" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q161" s="25"/>
       <c r="R161" s="26"/>
@@ -14326,16 +14315,16 @@
         <v>347</v>
       </c>
       <c r="F162" s="33" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="G162" s="33" t="s">
-        <v>922</v>
+        <v>910</v>
       </c>
       <c r="H162" s="33" t="s">
-        <v>923</v>
+        <v>911</v>
       </c>
       <c r="I162" s="33" t="s">
-        <v>924</v>
+        <v>912</v>
       </c>
       <c r="J162" s="34" t="s">
         <v>132</v>
@@ -14348,13 +14337,13 @@
         <v>132</v>
       </c>
       <c r="N162" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O162" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P162" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q162" s="25"/>
       <c r="R162" s="26"/>
@@ -14380,16 +14369,16 @@
         <v>349</v>
       </c>
       <c r="F163" s="33" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
       <c r="G163" s="33" t="s">
-        <v>925</v>
+        <v>913</v>
       </c>
       <c r="H163" s="33" t="s">
-        <v>926</v>
+        <v>914</v>
       </c>
       <c r="I163" s="33" t="s">
-        <v>927</v>
+        <v>915</v>
       </c>
       <c r="J163" s="34" t="s">
         <v>132</v>
@@ -14402,13 +14391,13 @@
         <v>132</v>
       </c>
       <c r="N163" s="34" t="s">
-        <v>953</v>
+        <v>941</v>
       </c>
       <c r="O163" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P163" s="34" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="Q163" s="25"/>
       <c r="R163" s="26"/>
@@ -14441,7 +14430,7 @@
         <v>841</v>
       </c>
       <c r="K164" s="34" t="s">
-        <v>947</v>
+        <v>935</v>
       </c>
       <c r="L164" s="25"/>
       <c r="M164" s="25"/>
@@ -14472,16 +14461,16 @@
         <v>353</v>
       </c>
       <c r="F165" s="33" t="s">
-        <v>928</v>
+        <v>916</v>
       </c>
       <c r="G165" s="33" t="s">
-        <v>928</v>
+        <v>916</v>
       </c>
       <c r="H165" s="33" t="s">
-        <v>929</v>
+        <v>917</v>
       </c>
       <c r="I165" s="33" t="s">
-        <v>930</v>
+        <v>918</v>
       </c>
       <c r="J165" s="34" t="s">
         <v>132</v>
@@ -14494,13 +14483,13 @@
         <v>132</v>
       </c>
       <c r="N165" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O165" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P165" s="34" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="Q165" s="25"/>
       <c r="R165" s="26"/>
@@ -14526,16 +14515,16 @@
         <v>355</v>
       </c>
       <c r="F166" s="33" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="G166" s="33" t="s">
-        <v>931</v>
+        <v>919</v>
       </c>
       <c r="H166" s="33" t="s">
-        <v>932</v>
+        <v>920</v>
       </c>
       <c r="I166" s="33" t="s">
-        <v>933</v>
+        <v>921</v>
       </c>
       <c r="J166" s="34" t="s">
         <v>132</v>
@@ -14548,13 +14537,13 @@
         <v>132</v>
       </c>
       <c r="N166" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O166" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P166" s="34" t="s">
-        <v>954</v>
+        <v>942</v>
       </c>
       <c r="Q166" s="25"/>
       <c r="R166" s="26"/>
@@ -14580,16 +14569,16 @@
         <v>357</v>
       </c>
       <c r="F167" s="33" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="G167" s="33" t="s">
-        <v>934</v>
+        <v>922</v>
       </c>
       <c r="H167" s="33" t="s">
-        <v>935</v>
+        <v>923</v>
       </c>
       <c r="I167" s="33" t="s">
-        <v>936</v>
+        <v>924</v>
       </c>
       <c r="J167" s="34" t="s">
         <v>132</v>
@@ -14602,13 +14591,13 @@
         <v>132</v>
       </c>
       <c r="N167" s="34" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="O167" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P167" s="34" t="s">
-        <v>955</v>
+        <v>943</v>
       </c>
       <c r="Q167" s="25"/>
       <c r="R167" s="26"/>
@@ -14634,16 +14623,16 @@
         <v>359</v>
       </c>
       <c r="F168" s="33" t="s">
-        <v>937</v>
+        <v>925</v>
       </c>
       <c r="G168" s="33" t="s">
-        <v>937</v>
+        <v>925</v>
       </c>
       <c r="H168" s="33" t="s">
-        <v>938</v>
+        <v>926</v>
       </c>
       <c r="I168" s="33" t="s">
-        <v>939</v>
+        <v>927</v>
       </c>
       <c r="J168" s="34" t="s">
         <v>132</v>
@@ -14656,13 +14645,13 @@
         <v>132</v>
       </c>
       <c r="N168" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O168" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P168" s="34" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="Q168" s="25"/>
       <c r="R168" s="26"/>
@@ -14695,7 +14684,7 @@
         <v>841</v>
       </c>
       <c r="K169" s="34" t="s">
-        <v>948</v>
+        <v>936</v>
       </c>
       <c r="L169" s="25"/>
       <c r="M169" s="25"/>
@@ -14726,16 +14715,16 @@
         <v>363</v>
       </c>
       <c r="F170" s="33" t="s">
-        <v>940</v>
+        <v>928</v>
       </c>
       <c r="G170" s="33" t="s">
-        <v>940</v>
+        <v>928</v>
       </c>
       <c r="H170" s="33" t="s">
-        <v>941</v>
+        <v>929</v>
       </c>
       <c r="I170" s="33" t="s">
-        <v>942</v>
+        <v>930</v>
       </c>
       <c r="J170" s="34" t="s">
         <v>132</v>
@@ -14748,13 +14737,13 @@
         <v>132</v>
       </c>
       <c r="N170" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O170" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P170" s="34" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="Q170" s="25"/>
       <c r="R170" s="26"/>
@@ -14787,7 +14776,7 @@
         <v>841</v>
       </c>
       <c r="K171" s="34" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
       <c r="L171" s="25"/>
       <c r="M171" s="25"/>
@@ -14825,7 +14814,7 @@
         <v>841</v>
       </c>
       <c r="K172" s="34" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="L172" s="25"/>
       <c r="M172" s="25"/>
@@ -14863,7 +14852,7 @@
         <v>841</v>
       </c>
       <c r="K173" s="34" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="L173" s="25"/>
       <c r="M173" s="25"/>
@@ -14901,7 +14890,7 @@
         <v>841</v>
       </c>
       <c r="K174" s="34" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
       <c r="L174" s="25"/>
       <c r="M174" s="25"/>
@@ -14939,7 +14928,7 @@
         <v>841</v>
       </c>
       <c r="K175" s="34" t="s">
-        <v>949</v>
+        <v>937</v>
       </c>
       <c r="L175" s="25"/>
       <c r="M175" s="25"/>
@@ -14970,16 +14959,16 @@
         <v>375</v>
       </c>
       <c r="F176" s="33" t="s">
-        <v>943</v>
+        <v>931</v>
       </c>
       <c r="G176" s="33" t="s">
-        <v>943</v>
+        <v>931</v>
       </c>
       <c r="H176" s="33" t="s">
-        <v>944</v>
+        <v>932</v>
       </c>
       <c r="I176" s="33" t="s">
-        <v>945</v>
+        <v>933</v>
       </c>
       <c r="J176" s="34" t="s">
         <v>132</v>
@@ -14992,13 +14981,13 @@
         <v>132</v>
       </c>
       <c r="N176" s="34" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="O176" s="34" t="s">
         <v>841</v>
       </c>
       <c r="P176" s="34" t="s">
-        <v>956</v>
+        <v>944</v>
       </c>
       <c r="Q176" s="25"/>
       <c r="R176" s="26"/>
@@ -15741,11 +15730,11 @@
       <c r="G198" s="24"/>
       <c r="H198" s="24"/>
       <c r="I198" s="24"/>
-      <c r="J198" s="25" t="s">
+      <c r="J198" s="34" t="s">
         <v>841</v>
       </c>
-      <c r="K198" s="25" t="s">
-        <v>1042</v>
+      <c r="K198" s="34" t="s">
+        <v>1033</v>
       </c>
       <c r="L198" s="25"/>
       <c r="M198" s="25"/>
@@ -21760,16 +21749,16 @@
         <v>771</v>
       </c>
       <c r="F375" s="33" t="s">
-        <v>988</v>
+        <v>976</v>
       </c>
       <c r="G375" s="33" t="s">
-        <v>988</v>
+        <v>976</v>
       </c>
       <c r="H375" s="33" t="s">
-        <v>989</v>
+        <v>977</v>
       </c>
       <c r="I375" s="33" t="s">
-        <v>990</v>
+        <v>978</v>
       </c>
       <c r="J375" s="34" t="s">
         <v>132</v>
@@ -21804,16 +21793,16 @@
         <v>773</v>
       </c>
       <c r="F376" s="33" t="s">
-        <v>957</v>
+        <v>945</v>
       </c>
       <c r="G376" s="33" t="s">
-        <v>957</v>
+        <v>945</v>
       </c>
       <c r="H376" s="33" t="s">
-        <v>958</v>
+        <v>946</v>
       </c>
       <c r="I376" s="33" t="s">
-        <v>959</v>
+        <v>947</v>
       </c>
       <c r="J376" s="25" t="s">
         <v>132</v>
@@ -21847,17 +21836,17 @@
       <c r="E377" s="35" t="s">
         <v>775</v>
       </c>
-      <c r="F377" s="36" t="s">
-        <v>847</v>
-      </c>
-      <c r="G377" s="36" t="s">
-        <v>847</v>
-      </c>
-      <c r="H377" s="36" t="s">
-        <v>848</v>
+      <c r="F377" s="33" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G377" s="33" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H377" s="33" t="s">
+        <v>1025</v>
       </c>
       <c r="I377" s="33" t="s">
-        <v>849</v>
+        <v>1026</v>
       </c>
       <c r="J377" s="34" t="s">
         <v>132</v>
@@ -21994,16 +21983,16 @@
         <v>783</v>
       </c>
       <c r="F381" s="33" t="s">
-        <v>904</v>
+        <v>1030</v>
       </c>
       <c r="G381" s="33" t="s">
-        <v>904</v>
+        <v>1030</v>
       </c>
       <c r="H381" s="33" t="s">
-        <v>905</v>
+        <v>1031</v>
       </c>
       <c r="I381" s="33" t="s">
-        <v>906</v>
+        <v>1032</v>
       </c>
       <c r="J381" s="34" t="s">
         <v>132</v>
@@ -22075,11 +22064,11 @@
       <c r="G383" s="24"/>
       <c r="H383" s="24"/>
       <c r="I383" s="24"/>
-      <c r="J383" s="25" t="s">
+      <c r="J383" s="34" t="s">
         <v>841</v>
       </c>
-      <c r="K383" s="25" t="s">
-        <v>1042</v>
+      <c r="K383" s="34" t="s">
+        <v>1033</v>
       </c>
       <c r="L383" s="25"/>
       <c r="M383" s="25"/>

</xml_diff>